<commit_message>
major 3d reconstruction enhancement
</commit_message>
<xml_diff>
--- a/display_detection/XSInstruments_pH.xlsx
+++ b/display_detection/XSInstruments_pH.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="2024-11-04" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="2025-04-29" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2025-04-30" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -826,6 +827,339 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>XSInstruments pH 50+ DHS S/N180356077</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Predicted Value</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="circle"/>
+            <size val="5"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'2025-04-30'!$C$2</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'2025-04-30'!$E$4</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Predicted Value</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="circle"/>
+            <size val="5"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'2025-04-30'!$J$2</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'2025-04-30'!$L$4</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>Predicted Value</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="circle"/>
+            <size val="5"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'2025-04-30'!$Q$2</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'2025-04-30'!$S$4</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>Predicted Value</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="circle"/>
+            <size val="5"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'2025-04-30'!$X$2</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'2025-04-30'!$Z$4</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Predicted Value</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="circle"/>
+            <size val="5"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'2025-04-30'!$AE$2</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'2025-04-30'!$AG$4</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Predicted Value</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="circle"/>
+            <size val="5"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'2025-04-30'!$AL$2</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'2025-04-30'!$AN$4</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Predicted Value</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="circle"/>
+            <size val="5"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'2025-04-30'!$AS$2</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'2025-04-30'!$AU$4</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Predicted Value</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="circle"/>
+            <size val="5"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'2025-04-30'!$AZ$2</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'2025-04-30'!$BB$4</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>pH</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -854,6 +1188,33 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -2602,7 +2963,7 @@
         <v>45776</v>
       </c>
       <c r="AS2" s="2" t="n">
-        <v>0.7225439343981481</v>
+        <v>0.7225439351851852</v>
       </c>
     </row>
     <row r="3">
@@ -3397,6 +3758,1064 @@
         </is>
       </c>
       <c r="AX11" t="n">
+        <v>0.8640649914741516</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:BE11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" s="1" t="n">
+        <v>45777</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0.5378098726851852</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>45777</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>0.5688517476851852</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>45777</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>0.5689745138888889</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <v>45777</v>
+      </c>
+      <c r="X2" s="2" t="n">
+        <v>0.5691420486111111</v>
+      </c>
+      <c r="AD2" s="1" t="n">
+        <v>45777</v>
+      </c>
+      <c r="AE2" s="2" t="n">
+        <v>0.5696062731481482</v>
+      </c>
+      <c r="AK2" s="1" t="n">
+        <v>45777</v>
+      </c>
+      <c r="AL2" s="2" t="n">
+        <v>0.5697759027777778</v>
+      </c>
+      <c r="AR2" s="1" t="n">
+        <v>45777</v>
+      </c>
+      <c r="AS2" s="2" t="n">
+        <v>0.569906412037037</v>
+      </c>
+      <c r="AY2" s="1" t="n">
+        <v>45777</v>
+      </c>
+      <c r="AZ2" s="2" t="n">
+        <v>0.5719710683101852</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>IDs</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Predicted values</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Confidence Interval</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>IDs</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Predicted values</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Confidence Interval</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>IDs</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Predicted values</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Confidence Interval</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>IDs</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Predicted values</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>Confidence Interval</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>IDs</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>Predicted values</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>Confidence Interval</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>IDs</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>Predicted values</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t>Confidence Interval</t>
+        </is>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t>IDs</t>
+        </is>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>Predicted values</t>
+        </is>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>Confidence Interval</t>
+        </is>
+      </c>
+      <c r="BA3" t="inlineStr">
+        <is>
+          <t>IDs</t>
+        </is>
+      </c>
+      <c r="BB3" t="inlineStr">
+        <is>
+          <t>Predicted values</t>
+        </is>
+      </c>
+      <c r="BC3" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="BD3" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>Confidence Interval</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9386836290359497</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4</v>
+      </c>
+      <c r="L4" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>0.9386836290359497</v>
+      </c>
+      <c r="R4" t="n">
+        <v>4</v>
+      </c>
+      <c r="S4" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
+        <v>0.9386836290359497</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.9386836290359497</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.9386836290359497</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="AP4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.9386836290359497</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="AV4" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AX4" t="n">
+        <v>0.9386836290359497</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>4</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="BC4" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="BD4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BE4" t="n">
+        <v>0.9386836290359497</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>0.6206219792366028</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3</v>
+      </c>
+      <c r="L5" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>0.6206219792366028</v>
+      </c>
+      <c r="R5" t="n">
+        <v>3</v>
+      </c>
+      <c r="S5" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="V5" t="n">
+        <v>0.6206219792366028</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.6206219792366028</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0.6206219792366028</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="AP5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0.6206219792366028</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="AV5" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="AW5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AX5" t="n">
+        <v>0.6206219792366028</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="BC5" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="BD5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE5" t="n">
+        <v>0.6206219792366028</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>0.9369140863418579</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>0.9369140863418579</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V6" t="n">
+        <v>0.9369140863418579</v>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.9369140863418579</v>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0.9369140863418579</v>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.9369140863418579</v>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.9369140863418579</v>
+      </c>
+      <c r="BD6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BE6" t="n">
+        <v>0.9369140863418579</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>0.8946381807327271</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
+        <v>0.8946381807327271</v>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="V7" t="n">
+        <v>0.8946381807327271</v>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.8946381807327271</v>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0.8946381807327271</v>
+      </c>
+      <c r="AP7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0.8946381807327271</v>
+      </c>
+      <c r="AW7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AX7" t="n">
+        <v>0.8946381807327271</v>
+      </c>
+      <c r="BD7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BE7" t="n">
+        <v>0.8946381807327271</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>0.8936176896095276</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
+        <v>0.8936176896095276</v>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="V8" t="n">
+        <v>0.8936176896095276</v>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AC8" t="n">
+        <v>0.8936176896095276</v>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AJ8" t="n">
+        <v>0.8936176896095276</v>
+      </c>
+      <c r="AP8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AQ8" t="n">
+        <v>0.8936176896095276</v>
+      </c>
+      <c r="AW8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AX8" t="n">
+        <v>0.8936176896095276</v>
+      </c>
+      <c r="BD8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BE8" t="n">
+        <v>0.8936176896095276</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>0.8272588849067688</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O9" t="n">
+        <v>0.8272588849067688</v>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="V9" t="n">
+        <v>0.8272588849067688</v>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AC9" t="n">
+        <v>0.8272588849067688</v>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0.8272588849067688</v>
+      </c>
+      <c r="AP9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ9" t="n">
+        <v>0.8272588849067688</v>
+      </c>
+      <c r="AW9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AX9" t="n">
+        <v>0.8272588849067688</v>
+      </c>
+      <c r="BD9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BE9" t="n">
+        <v>0.8272588849067688</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>0.6934510469436646</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="O10" t="n">
+        <v>0.6934510469436646</v>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="V10" t="n">
+        <v>0.6934510469436646</v>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AC10" t="n">
+        <v>0.6934510469436646</v>
+      </c>
+      <c r="AI10" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AJ10" t="n">
+        <v>0.6934510469436646</v>
+      </c>
+      <c r="AP10" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AQ10" t="n">
+        <v>0.6934510469436646</v>
+      </c>
+      <c r="AW10" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AX10" t="n">
+        <v>0.6934510469436646</v>
+      </c>
+      <c r="BD10" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE10" t="n">
+        <v>0.6934510469436646</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>0.8640649914741516</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>0.8640649914741516</v>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="V11" t="n">
+        <v>0.8640649914741516</v>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AC11" t="n">
+        <v>0.8640649914741516</v>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ11" t="n">
+        <v>0.8640649914741516</v>
+      </c>
+      <c r="AP11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ11" t="n">
+        <v>0.8640649914741516</v>
+      </c>
+      <c r="AW11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AX11" t="n">
+        <v>0.8640649914741516</v>
+      </c>
+      <c r="BD11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BE11" t="n">
         <v>0.8640649914741516</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cleaned up display detection
</commit_message>
<xml_diff>
--- a/display_detection/XSInstruments_pH.xlsx
+++ b/display_detection/XSInstruments_pH.xlsx
@@ -10,6 +10,7 @@
     <sheet name="2024-11-04" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="2025-04-29" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2025-04-30" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2025-05-22" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1160,6 +1161,153 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>XSInstruments pH 50+ DHS S/N180356077</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Predicted Value</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="circle"/>
+            <size val="5"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'2025-05-22'!$C$2</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'2025-05-22'!$E$4</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Predicted Value</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="circle"/>
+            <size val="5"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'2025-05-22'!$J$2</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'2025-05-22'!$L$4</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>pH</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -1215,6 +1363,33 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -3910,7 +4085,7 @@
         <v>45777</v>
       </c>
       <c r="AZ2" s="2" t="n">
-        <v>0.5719710683101852</v>
+        <v>0.5719710648148149</v>
       </c>
     </row>
     <row r="3">
@@ -4816,6 +4991,302 @@
         </is>
       </c>
       <c r="BE11" t="n">
+        <v>0.8640649914741516</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:O11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" s="1" t="n">
+        <v>45799</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0.3789717129629629</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>45799</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>0.3790324088541667</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>IDs</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Predicted values</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Confidence Interval</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>IDs</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Predicted values</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Confidence Interval</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9386836290359497</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4</v>
+      </c>
+      <c r="L4" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>0.9386836290359497</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>0.6206219792366028</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3</v>
+      </c>
+      <c r="L5" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>0.6206219792366028</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>0.9369140863418579</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>0.9369140863418579</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>0.8946381807327271</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
+        <v>0.8946381807327271</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>0.8936176896095276</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
+        <v>0.8936176896095276</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>0.8272588849067688</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O9" t="n">
+        <v>0.8272588849067688</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>0.6934510469436646</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="O10" t="n">
+        <v>0.6934510469436646</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>0.8640649914741516</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
         <v>0.8640649914741516</v>
       </c>
     </row>

</xml_diff>